<commit_message>
add choices and choice lists
</commit_message>
<xml_diff>
--- a/tests/assets/odk-example-form-1.xlsx
+++ b/tests/assets/odk-example-form-1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11110"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dave/Sites/holpa-platform/tests/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C5B7737-FCCB-3542-B1B0-2D4DC1030A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B801C23B-ED1A-8F4F-A2C3-126FEA97F92B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" tabRatio="321" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" tabRatio="321" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="67">
   <si>
     <t>type</t>
   </si>
@@ -230,6 +230,12 @@
   </si>
   <si>
     <t>Quel âge avez-vous ?</t>
+  </si>
+  <si>
+    <t>filter1</t>
+  </si>
+  <si>
+    <t>filter2</t>
   </si>
 </sst>
 </file>
@@ -406,7 +412,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -450,8 +456,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -920,7 +924,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="156" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="156" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
@@ -929,8 +933,8 @@
   <cols>
     <col min="1" max="1" width="35.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="25.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="34.83203125" style="21" customWidth="1"/>
-    <col min="4" max="4" width="34.83203125" style="23" customWidth="1"/>
+    <col min="3" max="3" width="34.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="34.83203125" style="21" customWidth="1"/>
     <col min="5" max="5" width="34.33203125" style="6" customWidth="1"/>
     <col min="6" max="7" width="18.5" style="1" customWidth="1"/>
     <col min="8" max="8" width="18.5" style="3" customWidth="1"/>
@@ -997,10 +1001,10 @@
       <c r="B2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="21" t="s">
         <v>62</v>
       </c>
       <c r="E2" s="6" t="s">
@@ -1014,10 +1018,10 @@
       <c r="B3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="21" t="s">
         <v>63</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -1031,10 +1035,10 @@
       <c r="B4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="21" t="s">
         <v>64</v>
       </c>
       <c r="E4" s="6" t="s">
@@ -1050,7 +1054,7 @@
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="B5" s="16"/>
-      <c r="C5" s="22"/>
+      <c r="C5" s="16"/>
       <c r="D5" s="18"/>
       <c r="E5" s="18"/>
       <c r="F5" s="16"/>
@@ -1059,7 +1063,7 @@
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="16"/>
       <c r="B6" s="16"/>
-      <c r="C6" s="22"/>
+      <c r="C6" s="16"/>
       <c r="D6" s="18"/>
       <c r="E6" s="18"/>
       <c r="F6" s="16"/>
@@ -1068,7 +1072,7 @@
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
       <c r="B7" s="16"/>
-      <c r="C7" s="22"/>
+      <c r="C7" s="16"/>
       <c r="D7" s="18"/>
       <c r="E7" s="17"/>
       <c r="F7" s="16"/>
@@ -1077,7 +1081,7 @@
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="16"/>
       <c r="B8" s="16"/>
-      <c r="C8" s="22"/>
+      <c r="C8" s="16"/>
       <c r="D8" s="18"/>
       <c r="E8" s="17"/>
       <c r="F8" s="16"/>
@@ -1086,7 +1090,7 @@
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="16"/>
       <c r="B9" s="16"/>
-      <c r="C9" s="22"/>
+      <c r="C9" s="16"/>
       <c r="D9" s="18"/>
       <c r="E9" s="17"/>
       <c r="F9" s="16"/>
@@ -1095,7 +1099,7 @@
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="16"/>
       <c r="B10" s="16"/>
-      <c r="C10" s="22"/>
+      <c r="C10" s="16"/>
       <c r="D10" s="18"/>
       <c r="E10" s="17"/>
       <c r="F10" s="16"/>
@@ -1104,7 +1108,7 @@
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="16"/>
       <c r="B11" s="16"/>
-      <c r="C11" s="22"/>
+      <c r="C11" s="16"/>
       <c r="D11" s="18"/>
       <c r="E11" s="17"/>
       <c r="F11" s="16"/>
@@ -1113,7 +1117,7 @@
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="16"/>
       <c r="B12" s="16"/>
-      <c r="C12" s="22"/>
+      <c r="C12" s="16"/>
       <c r="D12" s="18"/>
       <c r="E12" s="17"/>
       <c r="F12" s="16"/>
@@ -1122,7 +1126,7 @@
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="16"/>
       <c r="B13" s="16"/>
-      <c r="C13" s="22"/>
+      <c r="C13" s="16"/>
       <c r="D13" s="18"/>
       <c r="E13" s="17"/>
       <c r="F13" s="16"/>
@@ -1165,11 +1169,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView zoomScale="245" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="245" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1179,7 +1183,7 @@
     <col min="3" max="3" width="48.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="7" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="7" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>29</v>
       </c>
@@ -1189,8 +1193,14 @@
       <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1201,7 +1211,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -1212,7 +1222,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
         <v>28</v>
       </c>
@@ -1222,8 +1232,14 @@
       <c r="C6" s="15" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
         <v>28</v>
       </c>
@@ -1233,8 +1249,14 @@
       <c r="C7" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
         <v>28</v>
       </c>
@@ -1244,8 +1266,14 @@
       <c r="C8" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
         <v>28</v>
       </c>
@@ -1255,8 +1283,14 @@
       <c r="C9" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
         <v>28</v>
       </c>
@@ -1266,14 +1300,20 @@
       <c r="C10" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="15"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="15"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
         <v>43</v>
       </c>
@@ -1284,7 +1324,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
         <v>43</v>
       </c>
@@ -1295,7 +1335,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
         <v>43</v>
       </c>
@@ -1306,7 +1346,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
         <v>43</v>
       </c>
@@ -1376,7 +1416,7 @@
       </c>
       <c r="D2" s="19">
         <f ca="1">NOW()</f>
-        <v>45608.937544444445</v>
+        <v>45609.56917534722</v>
       </c>
       <c r="E2" t="s">
         <v>60</v>

</xml_diff>